<commit_message>
blad 1 even checken main
</commit_message>
<xml_diff>
--- a/IP.xlsx
+++ b/IP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ee38df677a9f564/Documenten/Maritieme techniek/Q4/IP-26-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_9A640D58C12CD2B6F91E7424993175CE37AA53CB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{459F7029-9C07-420A-8ABE-127201D6F508}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_9A640D58C12CD2B6F91E7424993175CE37AA53CB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C08EDB5B-85DB-49D8-B938-F11E389C115E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2604,20 +2604,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AD6DE1-4041-4B63-9CE0-C2DA987C4619}">
-  <dimension ref="A2:M178"/>
+  <dimension ref="A2:M157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A178"/>
+      <selection sqref="A1:A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>150</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2625,7 +2628,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>33.299999999999997</v>
+        <v>25.594000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2633,7 +2636,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>18</v>
+        <v>17.997</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2641,7 +2644,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>139.43</v>
+        <v>101.883</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2649,7 +2652,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>95.929000000000002</v>
+        <v>69.432000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2657,7 +2660,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>66.228999999999999</v>
+        <v>48.393999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2665,7 +2668,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>87.144000000000005</v>
+        <v>63.677</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2686,7 +2689,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>5.9969999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2694,7 +2697,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>5.9969999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2702,7 +2705,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>5.9969999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2723,7 +2726,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>25.149000000000001</v>
+        <v>21.966999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2739,13 +2742,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>123.642</v>
+        <v>90.290999999999997</v>
       </c>
       <c r="C18">
-        <v>-4.9950000000000001</v>
+        <v>-3.839</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>5.9969999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2758,7 +2761,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>7431.1930000000002</v>
+        <v>3406.05</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2766,7 +2769,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>46894.69</v>
+        <v>24884.823</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2774,13 +2777,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>88.096000000000004</v>
+        <v>64.138000000000005</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>3.69</v>
+        <v>3.8359999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2788,13 +2791,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>69.314999999999998</v>
+        <v>50.09</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>11.282999999999999</v>
+        <v>11.519</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2802,7 +2805,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.3291</v>
+        <v>0.28339999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2810,7 +2813,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.4783</v>
+        <v>0.41589999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2823,7 +2826,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>2002.11</v>
+        <v>1017.645</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2831,13 +2834,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>80.430999999999997</v>
+        <v>59.3</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>5.9969999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2845,13 +2848,13 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>90936.345000000001</v>
+        <v>23244.687000000002</v>
       </c>
       <c r="C29" s="6">
-        <v>1123300</v>
+        <v>293875.52500000002</v>
       </c>
       <c r="D29" s="6">
-        <v>1214200</v>
+        <v>317120.212</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2859,7 +2862,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>2417.6680000000001</v>
+        <v>1283.193</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2875,7 +2878,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>118.36199999999999</v>
+        <v>79.543999999999997</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2898,7 +2901,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>-2.8460000000000001</v>
+        <v>-2.0790000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2947,7 +2950,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>34.840000000000003</v>
+        <v>25.800999999999998</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -2955,167 +2958,167 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>39.470999999999997</v>
+        <v>29.106999999999999</v>
       </c>
       <c r="B45">
-        <v>8.1560000000000006</v>
+        <v>4.3330000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>44.100999999999999</v>
+        <v>32.414000000000001</v>
       </c>
       <c r="B46">
-        <v>20.417999999999999</v>
+        <v>11.52</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>48.731000000000002</v>
+        <v>35.72</v>
       </c>
       <c r="B47">
-        <v>34.146000000000001</v>
+        <v>19.879000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>53.362000000000002</v>
+        <v>39.026000000000003</v>
       </c>
       <c r="B48">
-        <v>48.600999999999999</v>
+        <v>28.873000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>57.991999999999997</v>
+        <v>42.332000000000001</v>
       </c>
       <c r="B49">
-        <v>63.271999999999998</v>
+        <v>38.152000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>62.622999999999998</v>
+        <v>45.639000000000003</v>
       </c>
       <c r="B50">
-        <v>77.688999999999993</v>
+        <v>47.414000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>67.253</v>
+        <v>48.945</v>
       </c>
       <c r="B51">
-        <v>91.316000000000003</v>
+        <v>56.341000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>71.882999999999996</v>
+        <v>52.250999999999998</v>
       </c>
       <c r="B52">
-        <v>103.429</v>
+        <v>64.516000000000005</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>76.513999999999996</v>
+        <v>55.557000000000002</v>
       </c>
       <c r="B53">
-        <v>112.925</v>
+        <v>71.281000000000006</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>81.144000000000005</v>
+        <v>58.863999999999997</v>
       </c>
       <c r="B54">
-        <v>118.14100000000001</v>
+        <v>75.507000000000005</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>85.774000000000001</v>
+        <v>62.17</v>
       </c>
       <c r="B55">
-        <v>118.36199999999999</v>
+        <v>77.245999999999995</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>90.405000000000001</v>
+        <v>65.475999999999999</v>
       </c>
       <c r="B56">
-        <v>117.056</v>
+        <v>79.13</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>95.034999999999997</v>
+        <v>68.781999999999996</v>
       </c>
       <c r="B57">
-        <v>114.88500000000001</v>
+        <v>79.543999999999997</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>99.665999999999997</v>
+        <v>72.088999999999999</v>
       </c>
       <c r="B58">
-        <v>111.39400000000001</v>
+        <v>77.391000000000005</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>104.29600000000001</v>
+        <v>75.394999999999996</v>
       </c>
       <c r="B59">
-        <v>106.095</v>
+        <v>72.772000000000006</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>108.926</v>
+        <v>78.700999999999993</v>
       </c>
       <c r="B60">
-        <v>98.447999999999993</v>
+        <v>66.429000000000002</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>113.557</v>
+        <v>82.007000000000005</v>
       </c>
       <c r="B61">
-        <v>88.031000000000006</v>
+        <v>58.447000000000003</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>118.187</v>
+        <v>85.313999999999993</v>
       </c>
       <c r="B62">
-        <v>74.599999999999994</v>
+        <v>48.283999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>122.818</v>
+        <v>88.62</v>
       </c>
       <c r="B63">
-        <v>57.768000000000001</v>
+        <v>35.082999999999998</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>127.44799999999999</v>
+        <v>91.926000000000002</v>
       </c>
       <c r="B64">
-        <v>35.896999999999998</v>
+        <v>17.393000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>132.078</v>
+        <v>95.233000000000004</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -3144,175 +3147,175 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>-2.8460000000000001</v>
+        <v>-2.0790000000000002</v>
       </c>
       <c r="B69">
-        <v>133.02799999999999</v>
+        <v>102.226</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>4.2969999999999997</v>
+        <v>2.968</v>
       </c>
       <c r="B70">
-        <v>168.786</v>
+        <v>127.51900000000001</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>11.44</v>
+        <v>8.016</v>
       </c>
       <c r="B71">
-        <v>204.67099999999999</v>
+        <v>152.774</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>18.582999999999998</v>
+        <v>13.064</v>
       </c>
       <c r="B72">
-        <v>240.55500000000001</v>
+        <v>177.89500000000001</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>25.725999999999999</v>
+        <v>18.111000000000001</v>
       </c>
       <c r="B73">
-        <v>276.291</v>
+        <v>202.78399999999999</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>32.869</v>
+        <v>23.158999999999999</v>
       </c>
       <c r="B74">
-        <v>311.69400000000002</v>
+        <v>227.32300000000001</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>40.012</v>
+        <v>28.206</v>
       </c>
       <c r="B75">
-        <v>346.517</v>
+        <v>251.36799999999999</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>47.154000000000003</v>
+        <v>33.253999999999998</v>
       </c>
       <c r="B76">
-        <v>380.40699999999998</v>
+        <v>274.72800000000001</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>54.296999999999997</v>
+        <v>38.302</v>
       </c>
       <c r="B77">
-        <v>412.82799999999997</v>
+        <v>297.137</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>61.44</v>
+        <v>43.348999999999997</v>
       </c>
       <c r="B78">
-        <v>442.9</v>
+        <v>318.185</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>68.582999999999998</v>
+        <v>48.396999999999998</v>
       </c>
       <c r="B79">
-        <v>469.00900000000001</v>
+        <v>337.14</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>75.725999999999999</v>
+        <v>53.445</v>
       </c>
       <c r="B80">
-        <v>487.76799999999997</v>
+        <v>352.44799999999998</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>82.869</v>
+        <v>58.491999999999997</v>
       </c>
       <c r="B81">
-        <v>491.70600000000002</v>
+        <v>359.928</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>90.012</v>
+        <v>63.54</v>
       </c>
       <c r="B82">
-        <v>478.90899999999999</v>
+        <v>353.221</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>97.153999999999996</v>
+        <v>68.587000000000003</v>
       </c>
       <c r="B83">
-        <v>454.48899999999998</v>
+        <v>331.08499999999998</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>104.297</v>
+        <v>73.635000000000005</v>
       </c>
       <c r="B84">
-        <v>414.92899999999997</v>
+        <v>300.39</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>111.44</v>
+        <v>78.683000000000007</v>
       </c>
       <c r="B85">
-        <v>359.08</v>
+        <v>266.00599999999997</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>118.583</v>
+        <v>83.73</v>
       </c>
       <c r="B86">
-        <v>285.75599999999997</v>
+        <v>226.17</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>125.726</v>
+        <v>88.778000000000006</v>
       </c>
       <c r="B87">
-        <v>190.76400000000001</v>
+        <v>175.953</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>132.869</v>
+        <v>93.825999999999993</v>
       </c>
       <c r="B88">
-        <v>57.351999999999997</v>
+        <v>106.474</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>140.012</v>
+        <v>98.873000000000005</v>
       </c>
       <c r="B89">
-        <v>17.103999999999999</v>
+        <v>37.396999999999998</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>147.154</v>
+        <v>103.92100000000001</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -3354,7 +3357,7 @@
         <v>46</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
@@ -3362,7 +3365,7 @@
         <v>40</v>
       </c>
       <c r="B97">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
@@ -3402,34 +3405,34 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>-2.8460000000000001</v>
+        <v>-2.0790000000000002</v>
       </c>
       <c r="B99">
-        <v>66.861000000000004</v>
+        <v>52.798000000000002</v>
       </c>
       <c r="C99">
-        <v>133.02799999999999</v>
+        <v>0.158</v>
       </c>
       <c r="D99">
-        <v>-2.8460000000000001</v>
+        <v>-2.0790000000000002</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
       <c r="F99">
-        <v>15.663</v>
+        <v>15.913</v>
       </c>
       <c r="G99">
-        <v>8129.7629999999999</v>
+        <v>9.4390000000000001</v>
       </c>
       <c r="H99">
-        <v>285.57900000000001</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="I99">
-        <v>7844.1840000000002</v>
+        <v>8.6229999999999993</v>
       </c>
       <c r="J99">
-        <v>12.516</v>
+        <v>12.510999999999999</v>
       </c>
       <c r="K99">
         <v>18</v>
@@ -3437,34 +3440,34 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>-2.8460000000000001</v>
+        <v>2.968</v>
       </c>
       <c r="B100">
-        <v>66.861000000000004</v>
+        <v>54.908000000000001</v>
       </c>
       <c r="C100">
-        <v>133.02799999999999</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D100">
-        <v>-2.8460000000000001</v>
+        <v>2.968</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="F100">
-        <v>15.663</v>
+        <v>15.427</v>
       </c>
       <c r="G100">
-        <v>8129.7629999999999</v>
+        <v>10.702999999999999</v>
       </c>
       <c r="H100">
-        <v>285.57900000000001</v>
+        <v>1.252</v>
       </c>
       <c r="I100">
-        <v>7844.1840000000002</v>
+        <v>9.4510000000000005</v>
       </c>
       <c r="J100">
-        <v>12.516</v>
+        <v>11.305</v>
       </c>
       <c r="K100">
         <v>18</v>
@@ -3472,34 +3475,34 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>4.2969999999999997</v>
+        <v>8.016</v>
       </c>
       <c r="B101">
-        <v>69.108000000000004</v>
+        <v>56.991</v>
       </c>
       <c r="C101">
-        <v>168.786</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="D101">
-        <v>4.2969999999999997</v>
+        <v>8.016</v>
       </c>
       <c r="E101">
         <v>0</v>
       </c>
       <c r="F101">
-        <v>15.09</v>
+        <v>14.944000000000001</v>
       </c>
       <c r="G101">
-        <v>10926.18</v>
+        <v>12.063000000000001</v>
       </c>
       <c r="H101">
-        <v>555.18100000000004</v>
+        <v>1.784</v>
       </c>
       <c r="I101">
-        <v>10371</v>
+        <v>10.278</v>
       </c>
       <c r="J101">
-        <v>11.25</v>
+        <v>10.106999999999999</v>
       </c>
       <c r="K101">
         <v>18</v>
@@ -3507,34 +3510,34 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>4.2969999999999997</v>
+        <v>13.064</v>
       </c>
       <c r="B102">
-        <v>69.108000000000004</v>
+        <v>59.054000000000002</v>
       </c>
       <c r="C102">
-        <v>168.786</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="D102">
-        <v>4.2969999999999997</v>
+        <v>13.064</v>
       </c>
       <c r="E102">
         <v>0</v>
       </c>
       <c r="F102">
-        <v>15.09</v>
+        <v>14.465999999999999</v>
       </c>
       <c r="G102">
-        <v>10926.18</v>
+        <v>13.519</v>
       </c>
       <c r="H102">
-        <v>555.18100000000004</v>
+        <v>2.4089999999999998</v>
       </c>
       <c r="I102">
-        <v>10371</v>
+        <v>11.11</v>
       </c>
       <c r="J102">
-        <v>11.25</v>
+        <v>8.9209999999999994</v>
       </c>
       <c r="K102">
         <v>18</v>
@@ -3542,34 +3545,34 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>11.44</v>
+        <v>18.111000000000001</v>
       </c>
       <c r="B103">
-        <v>71.340999999999994</v>
+        <v>61.091000000000001</v>
       </c>
       <c r="C103">
-        <v>204.67099999999999</v>
+        <v>0.183</v>
       </c>
       <c r="D103">
-        <v>11.44</v>
+        <v>18.111000000000001</v>
       </c>
       <c r="E103">
         <v>0</v>
       </c>
       <c r="F103">
-        <v>14.522</v>
+        <v>13.996</v>
       </c>
       <c r="G103">
-        <v>13935.403</v>
+        <v>15.068</v>
       </c>
       <c r="H103">
-        <v>953.93399999999997</v>
+        <v>3.1230000000000002</v>
       </c>
       <c r="I103">
-        <v>12981.468999999999</v>
+        <v>11.945</v>
       </c>
       <c r="J103">
-        <v>9.9949999999999992</v>
+        <v>7.7480000000000002</v>
       </c>
       <c r="K103">
         <v>18</v>
@@ -3577,34 +3580,34 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>11.44</v>
+        <v>23.158999999999999</v>
       </c>
       <c r="B104">
-        <v>71.340999999999994</v>
+        <v>63.097000000000001</v>
       </c>
       <c r="C104">
-        <v>204.67099999999999</v>
+        <v>0.189</v>
       </c>
       <c r="D104">
-        <v>11.44</v>
+        <v>23.158999999999999</v>
       </c>
       <c r="E104">
         <v>0</v>
       </c>
       <c r="F104">
-        <v>14.522</v>
+        <v>13.534000000000001</v>
       </c>
       <c r="G104">
-        <v>13935.403</v>
+        <v>16.698</v>
       </c>
       <c r="H104">
-        <v>953.93399999999997</v>
+        <v>3.919</v>
       </c>
       <c r="I104">
-        <v>12981.468999999999</v>
+        <v>12.779</v>
       </c>
       <c r="J104">
-        <v>9.9949999999999992</v>
+        <v>6.5919999999999996</v>
       </c>
       <c r="K104">
         <v>18</v>
@@ -3612,34 +3615,34 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>18.582999999999998</v>
+        <v>28.206</v>
       </c>
       <c r="B105">
-        <v>73.570999999999998</v>
+        <v>65.058000000000007</v>
       </c>
       <c r="C105">
-        <v>240.55500000000001</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="D105">
-        <v>18.582999999999998</v>
+        <v>28.206</v>
       </c>
       <c r="E105">
         <v>0</v>
       </c>
       <c r="F105">
-        <v>13.962</v>
+        <v>13.082000000000001</v>
       </c>
       <c r="G105">
-        <v>17167.402999999998</v>
+        <v>18.398</v>
       </c>
       <c r="H105">
-        <v>1502.5119999999999</v>
+        <v>4.7910000000000004</v>
       </c>
       <c r="I105">
-        <v>15664.891</v>
+        <v>13.606999999999999</v>
       </c>
       <c r="J105">
-        <v>8.7530000000000001</v>
+        <v>5.4550000000000001</v>
       </c>
       <c r="K105">
         <v>18</v>
@@ -3647,34 +3650,34 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>18.582999999999998</v>
+        <v>33.253999999999998</v>
       </c>
       <c r="B106">
-        <v>73.570999999999998</v>
+        <v>66.959000000000003</v>
       </c>
       <c r="C106">
-        <v>240.55500000000001</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="D106">
-        <v>18.582999999999998</v>
+        <v>33.253999999999998</v>
       </c>
       <c r="E106">
         <v>0</v>
       </c>
       <c r="F106">
-        <v>13.962</v>
+        <v>12.644</v>
       </c>
       <c r="G106">
-        <v>17167.402999999998</v>
+        <v>20.146000000000001</v>
       </c>
       <c r="H106">
-        <v>1502.5119999999999</v>
+        <v>5.7249999999999996</v>
       </c>
       <c r="I106">
-        <v>15664.891</v>
+        <v>14.420999999999999</v>
       </c>
       <c r="J106">
-        <v>8.7530000000000001</v>
+        <v>4.3470000000000004</v>
       </c>
       <c r="K106">
         <v>18</v>
@@ -3682,34 +3685,34 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>25.725999999999999</v>
+        <v>38.302</v>
       </c>
       <c r="B107">
-        <v>75.790000000000006</v>
+        <v>68.775000000000006</v>
       </c>
       <c r="C107">
-        <v>276.291</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="D107">
-        <v>25.725999999999999</v>
+        <v>38.302</v>
       </c>
       <c r="E107">
         <v>0</v>
       </c>
       <c r="F107">
-        <v>13.411</v>
+        <v>12.215999999999999</v>
       </c>
       <c r="G107">
-        <v>20626.267</v>
+        <v>21.945</v>
       </c>
       <c r="H107">
-        <v>2217.6370000000002</v>
+        <v>6.7130000000000001</v>
       </c>
       <c r="I107">
-        <v>18408.63</v>
+        <v>15.231999999999999</v>
       </c>
       <c r="J107">
-        <v>7.5289999999999999</v>
+        <v>3.2850000000000001</v>
       </c>
       <c r="K107">
         <v>18</v>
@@ -3717,34 +3720,34 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>25.725999999999999</v>
+        <v>43.348999999999997</v>
       </c>
       <c r="B108">
-        <v>75.790000000000006</v>
+        <v>70.468000000000004</v>
       </c>
       <c r="C108">
-        <v>276.291</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="D108">
-        <v>25.725999999999999</v>
+        <v>43.348999999999997</v>
       </c>
       <c r="E108">
         <v>0</v>
       </c>
       <c r="F108">
-        <v>13.411</v>
+        <v>11.817</v>
       </c>
       <c r="G108">
-        <v>20626.267</v>
+        <v>23.678999999999998</v>
       </c>
       <c r="H108">
-        <v>2217.6370000000002</v>
+        <v>7.7110000000000003</v>
       </c>
       <c r="I108">
-        <v>18408.63</v>
+        <v>15.968</v>
       </c>
       <c r="J108">
-        <v>7.5289999999999999</v>
+        <v>2.2890000000000001</v>
       </c>
       <c r="K108">
         <v>18</v>
@@ -3752,34 +3755,34 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>32.869</v>
+        <v>48.396999999999998</v>
       </c>
       <c r="B109">
-        <v>77.983999999999995</v>
+        <v>71.966999999999999</v>
       </c>
       <c r="C109">
-        <v>311.69400000000002</v>
+        <v>0.216</v>
       </c>
       <c r="D109">
-        <v>32.869</v>
+        <v>48.396999999999998</v>
       </c>
       <c r="E109">
         <v>0</v>
       </c>
       <c r="F109">
-        <v>12.872999999999999</v>
+        <v>11.45</v>
       </c>
       <c r="G109">
-        <v>24306.15</v>
+        <v>25.286000000000001</v>
       </c>
       <c r="H109">
-        <v>3110.5659999999998</v>
+        <v>8.6790000000000003</v>
       </c>
       <c r="I109">
-        <v>21195.583999999999</v>
+        <v>16.606999999999999</v>
       </c>
       <c r="J109">
-        <v>6.327</v>
+        <v>1.39</v>
       </c>
       <c r="K109">
         <v>18</v>
@@ -3787,34 +3790,34 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>32.869</v>
+        <v>53.445</v>
       </c>
       <c r="B110">
-        <v>77.983999999999995</v>
+        <v>73.122</v>
       </c>
       <c r="C110">
-        <v>311.69400000000002</v>
+        <v>0.219</v>
       </c>
       <c r="D110">
-        <v>32.869</v>
+        <v>53.445</v>
       </c>
       <c r="E110">
         <v>0</v>
       </c>
       <c r="F110">
-        <v>12.872999999999999</v>
+        <v>11.135999999999999</v>
       </c>
       <c r="G110">
-        <v>24306.15</v>
+        <v>26.588000000000001</v>
       </c>
       <c r="H110">
-        <v>3110.5659999999998</v>
+        <v>9.5289999999999999</v>
       </c>
       <c r="I110">
-        <v>21195.583999999999</v>
+        <v>17.059000000000001</v>
       </c>
       <c r="J110">
-        <v>6.327</v>
+        <v>0.65</v>
       </c>
       <c r="K110">
         <v>18</v>
@@ -3822,34 +3825,34 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>40.012</v>
+        <v>58.491999999999997</v>
       </c>
       <c r="B111">
-        <v>80.132000000000005</v>
+        <v>73.510000000000005</v>
       </c>
       <c r="C111">
-        <v>346.517</v>
+        <v>0.221</v>
       </c>
       <c r="D111">
-        <v>40.012</v>
+        <v>58.491999999999997</v>
       </c>
       <c r="E111">
         <v>0</v>
       </c>
       <c r="F111">
-        <v>12.349</v>
+        <v>10.916</v>
       </c>
       <c r="G111">
-        <v>28185.690999999999</v>
+        <v>27.071999999999999</v>
       </c>
       <c r="H111">
-        <v>4184.8050000000003</v>
+        <v>10.042</v>
       </c>
       <c r="I111">
-        <v>24000.885999999999</v>
+        <v>17.03</v>
       </c>
       <c r="J111">
-        <v>5.1539999999999999</v>
+        <v>0.223</v>
       </c>
       <c r="K111">
         <v>18</v>
@@ -3857,34 +3860,34 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>40.012</v>
+        <v>63.54</v>
       </c>
       <c r="B112">
-        <v>80.132000000000005</v>
+        <v>72.353999999999999</v>
       </c>
       <c r="C112">
-        <v>346.517</v>
+        <v>0.217</v>
       </c>
       <c r="D112">
-        <v>40.012</v>
+        <v>63.54</v>
       </c>
       <c r="E112">
         <v>0</v>
       </c>
       <c r="F112">
-        <v>12.349</v>
+        <v>10.771000000000001</v>
       </c>
       <c r="G112">
-        <v>28185.690999999999</v>
+        <v>25.856999999999999</v>
       </c>
       <c r="H112">
-        <v>4184.8050000000003</v>
+        <v>10.039</v>
       </c>
       <c r="I112">
-        <v>24000.885999999999</v>
+        <v>15.818</v>
       </c>
       <c r="J112">
-        <v>5.1539999999999999</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="K112">
         <v>18</v>
@@ -3892,34 +3895,34 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>47.154000000000003</v>
+        <v>68.587000000000003</v>
       </c>
       <c r="B113">
-        <v>82.207999999999998</v>
+        <v>69.647000000000006</v>
       </c>
       <c r="C113">
-        <v>380.40699999999998</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="D113">
-        <v>47.154000000000003</v>
+        <v>68.587000000000003</v>
       </c>
       <c r="E113">
         <v>0</v>
       </c>
       <c r="F113">
-        <v>11.843999999999999</v>
+        <v>10.56</v>
       </c>
       <c r="G113">
-        <v>32218.976999999999</v>
+        <v>23</v>
       </c>
       <c r="H113">
-        <v>5432.41</v>
+        <v>9.8369999999999997</v>
       </c>
       <c r="I113">
-        <v>26786.566999999999</v>
+        <v>13.162000000000001</v>
       </c>
       <c r="J113">
-        <v>4.0179999999999998</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="K113">
         <v>18</v>
@@ -3927,34 +3930,34 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>47.154000000000003</v>
+        <v>73.635000000000005</v>
       </c>
       <c r="B114">
-        <v>82.207999999999998</v>
+        <v>66.424999999999997</v>
       </c>
       <c r="C114">
-        <v>380.40699999999998</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="D114">
-        <v>47.154000000000003</v>
+        <v>73.635000000000005</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="F114">
-        <v>11.843999999999999</v>
+        <v>10.452999999999999</v>
       </c>
       <c r="G114">
-        <v>32218.976999999999</v>
+        <v>19.792000000000002</v>
       </c>
       <c r="H114">
-        <v>5432.41</v>
+        <v>9.3919999999999995</v>
       </c>
       <c r="I114">
-        <v>26786.566999999999</v>
+        <v>10.4</v>
       </c>
       <c r="J114">
-        <v>4.0179999999999998</v>
+        <v>-2E-3</v>
       </c>
       <c r="K114">
         <v>18</v>
@@ -3962,34 +3965,34 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>54.296999999999997</v>
+        <v>78.683000000000007</v>
       </c>
       <c r="B115">
-        <v>84.174000000000007</v>
+        <v>63.017000000000003</v>
       </c>
       <c r="C115">
-        <v>412.82799999999997</v>
+        <v>0.189</v>
       </c>
       <c r="D115">
-        <v>54.296999999999997</v>
+        <v>78.683000000000007</v>
       </c>
       <c r="E115">
         <v>0</v>
       </c>
       <c r="F115">
-        <v>11.364000000000001</v>
+        <v>10.473000000000001</v>
       </c>
       <c r="G115">
-        <v>36319.148999999998</v>
+        <v>16.704000000000001</v>
       </c>
       <c r="H115">
-        <v>6827.4920000000002</v>
+        <v>8.6869999999999994</v>
       </c>
       <c r="I115">
-        <v>29491.656999999999</v>
+        <v>8.0169999999999995</v>
       </c>
       <c r="J115">
-        <v>2.9340000000000002</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K115">
         <v>18</v>
@@ -3997,34 +4000,34 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>54.296999999999997</v>
+        <v>83.73</v>
       </c>
       <c r="B116">
-        <v>84.174000000000007</v>
+        <v>59.076000000000001</v>
       </c>
       <c r="C116">
-        <v>412.82799999999997</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="D116">
-        <v>54.296999999999997</v>
+        <v>83.73</v>
       </c>
       <c r="E116">
         <v>0</v>
       </c>
       <c r="F116">
-        <v>11.364000000000001</v>
+        <v>10.608000000000001</v>
       </c>
       <c r="G116">
-        <v>36319.148999999998</v>
+        <v>13.531000000000001</v>
       </c>
       <c r="H116">
-        <v>6827.4920000000002</v>
+        <v>7.7149999999999999</v>
       </c>
       <c r="I116">
-        <v>29491.656999999999</v>
+        <v>5.8170000000000002</v>
       </c>
       <c r="J116">
-        <v>2.9340000000000002</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="K116">
         <v>18</v>
@@ -4032,34 +4035,34 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>61.44</v>
+        <v>88.778000000000006</v>
       </c>
       <c r="B117">
-        <v>85.966999999999999</v>
+        <v>53.747999999999998</v>
       </c>
       <c r="C117">
-        <v>442.9</v>
+        <v>0.161</v>
       </c>
       <c r="D117">
-        <v>61.44</v>
+        <v>88.778000000000006</v>
       </c>
       <c r="E117">
         <v>0</v>
       </c>
       <c r="F117">
-        <v>10.917999999999999</v>
+        <v>11.009</v>
       </c>
       <c r="G117">
-        <v>40325.281999999999</v>
+        <v>9.9260000000000002</v>
       </c>
       <c r="H117">
-        <v>8313.73</v>
+        <v>6.1920000000000002</v>
       </c>
       <c r="I117">
-        <v>32011.552</v>
+        <v>3.734</v>
       </c>
       <c r="J117">
-        <v>1.925</v>
+        <v>0.69</v>
       </c>
       <c r="K117">
         <v>18</v>
@@ -4067,34 +4070,34 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>61.44</v>
+        <v>93.825999999999993</v>
       </c>
       <c r="B118">
-        <v>85.966999999999999</v>
+        <v>43.088000000000001</v>
       </c>
       <c r="C118">
-        <v>442.9</v>
+        <v>0.129</v>
       </c>
       <c r="D118">
-        <v>61.44</v>
+        <v>93.825999999999993</v>
       </c>
       <c r="E118">
         <v>0</v>
       </c>
       <c r="F118">
-        <v>10.917999999999999</v>
+        <v>12.552</v>
       </c>
       <c r="G118">
-        <v>40325.281999999999</v>
+        <v>4.9569999999999999</v>
       </c>
       <c r="H118">
-        <v>8313.73</v>
+        <v>3.1120000000000001</v>
       </c>
       <c r="I118">
-        <v>32011.552</v>
+        <v>1.8440000000000001</v>
       </c>
       <c r="J118">
-        <v>1.925</v>
+        <v>3.8650000000000002</v>
       </c>
       <c r="K118">
         <v>18</v>
@@ -4102,34 +4105,34 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>68.582999999999998</v>
+        <v>98.873000000000005</v>
       </c>
       <c r="B119">
-        <v>87.471999999999994</v>
+        <v>24.943000000000001</v>
       </c>
       <c r="C119">
-        <v>469.00900000000001</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="D119">
-        <v>68.582999999999998</v>
+        <v>98.873000000000005</v>
       </c>
       <c r="E119">
         <v>0</v>
       </c>
       <c r="F119">
-        <v>10.523</v>
+        <v>15.510999999999999</v>
       </c>
       <c r="G119">
-        <v>43926.307999999997</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="H119">
-        <v>9777.2800000000007</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="I119">
-        <v>34149.027999999998</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="J119">
-        <v>1.036</v>
+        <v>11.237</v>
       </c>
       <c r="K119">
         <v>18</v>
@@ -4137,1092 +4140,357 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>68.582999999999998</v>
+        <v>103.92100000000001</v>
       </c>
       <c r="B120">
-        <v>87.471999999999994</v>
+        <v>0</v>
       </c>
       <c r="C120">
-        <v>469.00900000000001</v>
+        <v>0</v>
       </c>
       <c r="D120">
-        <v>68.582999999999998</v>
+        <v>103.92100000000001</v>
       </c>
       <c r="E120">
         <v>0</v>
       </c>
       <c r="F120">
-        <v>10.523</v>
+        <v>17.995999999999999</v>
       </c>
       <c r="G120">
-        <v>43926.307999999997</v>
+        <v>0</v>
       </c>
       <c r="H120">
-        <v>9777.2800000000007</v>
+        <v>0</v>
       </c>
       <c r="I120">
-        <v>34149.027999999998</v>
+        <v>0</v>
       </c>
       <c r="J120">
-        <v>1.036</v>
+        <v>0</v>
       </c>
       <c r="K120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>59</v>
+      </c>
+      <c r="B122">
+        <v>101.883</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>60</v>
+      </c>
+      <c r="B123">
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>61</v>
+      </c>
+      <c r="B124">
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A121">
-        <v>75.725999999999999</v>
-      </c>
-      <c r="B121">
-        <v>88.438000000000002</v>
-      </c>
-      <c r="C121">
-        <v>487.76799999999997</v>
-      </c>
-      <c r="D121">
-        <v>75.725999999999999</v>
-      </c>
-      <c r="E121">
-        <v>0</v>
-      </c>
-      <c r="F121">
-        <v>10.214</v>
-      </c>
-      <c r="G121">
-        <v>46460.464</v>
-      </c>
-      <c r="H121">
-        <v>10980.885</v>
-      </c>
-      <c r="I121">
-        <v>35479.578999999998</v>
-      </c>
-      <c r="J121">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="K121">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A122">
-        <v>75.725999999999999</v>
-      </c>
-      <c r="B122">
-        <v>88.438000000000002</v>
-      </c>
-      <c r="C122">
-        <v>487.76799999999997</v>
-      </c>
-      <c r="D122">
-        <v>75.725999999999999</v>
-      </c>
-      <c r="E122">
-        <v>0</v>
-      </c>
-      <c r="F122">
-        <v>10.214</v>
-      </c>
-      <c r="G122">
-        <v>46460.464</v>
-      </c>
-      <c r="H122">
-        <v>10980.885</v>
-      </c>
-      <c r="I122">
-        <v>35479.578999999998</v>
-      </c>
-      <c r="J122">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="K122">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A123">
-        <v>82.869</v>
-      </c>
-      <c r="B123">
-        <v>88.278000000000006</v>
-      </c>
-      <c r="C123">
-        <v>491.70600000000002</v>
-      </c>
-      <c r="D123">
-        <v>82.869</v>
-      </c>
-      <c r="E123">
-        <v>0</v>
-      </c>
-      <c r="F123">
-        <v>10.058</v>
-      </c>
-      <c r="G123">
-        <v>46471.557999999997</v>
-      </c>
-      <c r="H123">
-        <v>11449.144</v>
-      </c>
-      <c r="I123">
-        <v>35022.413999999997</v>
-      </c>
-      <c r="J123">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="K123">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A124">
-        <v>82.869</v>
-      </c>
-      <c r="B124">
-        <v>88.278000000000006</v>
-      </c>
-      <c r="C124">
-        <v>491.70600000000002</v>
-      </c>
-      <c r="D124">
-        <v>82.869</v>
-      </c>
-      <c r="E124">
-        <v>0</v>
-      </c>
-      <c r="F124">
-        <v>10.058</v>
-      </c>
-      <c r="G124">
-        <v>46471.557999999997</v>
-      </c>
-      <c r="H124">
-        <v>11449.144</v>
-      </c>
-      <c r="I124">
-        <v>35022.413999999997</v>
-      </c>
-      <c r="J124">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="K124">
-        <v>18</v>
-      </c>
-    </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A125">
-        <v>90.012</v>
+      <c r="A125" t="s">
+        <v>62</v>
       </c>
       <c r="B125">
-        <v>86.703999999999994</v>
-      </c>
-      <c r="C125">
-        <v>478.90899999999999</v>
-      </c>
-      <c r="D125">
-        <v>90.012</v>
-      </c>
-      <c r="E125">
-        <v>0</v>
-      </c>
-      <c r="F125">
-        <v>10.016999999999999</v>
-      </c>
-      <c r="G125">
-        <v>43342.313000000002</v>
-      </c>
-      <c r="H125">
-        <v>11164.501</v>
-      </c>
-      <c r="I125">
-        <v>32177.812000000002</v>
-      </c>
-      <c r="J125">
-        <v>0.109</v>
-      </c>
-      <c r="K125">
-        <v>18</v>
+        <v>5.9969999999999999</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A126">
-        <v>90.012</v>
+      <c r="A126" t="s">
+        <v>63</v>
       </c>
       <c r="B126">
-        <v>86.703999999999994</v>
-      </c>
-      <c r="C126">
-        <v>478.90899999999999</v>
-      </c>
-      <c r="D126">
-        <v>90.012</v>
-      </c>
-      <c r="E126">
-        <v>0</v>
-      </c>
-      <c r="F126">
-        <v>10.016999999999999</v>
-      </c>
-      <c r="G126">
-        <v>43342.313000000002</v>
-      </c>
-      <c r="H126">
-        <v>11164.501</v>
-      </c>
-      <c r="I126">
-        <v>32177.812000000002</v>
-      </c>
-      <c r="J126">
-        <v>0.109</v>
-      </c>
-      <c r="K126">
-        <v>18</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A127">
-        <v>97.153999999999996</v>
+      <c r="A127" t="s">
+        <v>64</v>
       </c>
       <c r="B127">
-        <v>84.018000000000001</v>
-      </c>
-      <c r="C127">
-        <v>454.48899999999998</v>
-      </c>
-      <c r="D127">
-        <v>97.153999999999996</v>
-      </c>
-      <c r="E127">
-        <v>0</v>
-      </c>
-      <c r="F127">
-        <v>9.9700000000000006</v>
-      </c>
-      <c r="G127">
-        <v>37954.69</v>
-      </c>
-      <c r="H127">
-        <v>10662.816000000001</v>
-      </c>
-      <c r="I127">
-        <v>27291.874</v>
-      </c>
-      <c r="J127">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="K127">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A128">
-        <v>97.153999999999996</v>
+      <c r="A128" t="s">
+        <v>65</v>
       </c>
       <c r="B128">
-        <v>84.018000000000001</v>
-      </c>
-      <c r="C128">
-        <v>454.48899999999998</v>
-      </c>
-      <c r="D128">
-        <v>97.153999999999996</v>
-      </c>
-      <c r="E128">
-        <v>0</v>
-      </c>
-      <c r="F128">
-        <v>9.9700000000000006</v>
-      </c>
-      <c r="G128">
-        <v>37954.69</v>
-      </c>
-      <c r="H128">
-        <v>10662.816000000001</v>
-      </c>
-      <c r="I128">
-        <v>27291.874</v>
-      </c>
-      <c r="J128">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="K128">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A129">
-        <v>104.297</v>
+        <v>15282.407999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>66</v>
       </c>
       <c r="B129">
-        <v>80.150999999999996</v>
-      </c>
-      <c r="C129">
-        <v>414.92899999999997</v>
-      </c>
-      <c r="D129">
-        <v>104.297</v>
-      </c>
-      <c r="E129">
-        <v>0</v>
-      </c>
-      <c r="F129">
-        <v>9.9380000000000006</v>
-      </c>
-      <c r="G129">
-        <v>30479.712</v>
-      </c>
-      <c r="H129">
-        <v>9915.99</v>
-      </c>
-      <c r="I129">
-        <v>20563.722000000002</v>
-      </c>
-      <c r="J129">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="K129">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A130">
-        <v>104.297</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>7</v>
       </c>
       <c r="B130">
-        <v>80.150999999999996</v>
-      </c>
-      <c r="C130">
-        <v>414.92899999999997</v>
-      </c>
-      <c r="D130">
-        <v>104.297</v>
-      </c>
-      <c r="E130">
-        <v>0</v>
-      </c>
-      <c r="F130">
-        <v>9.9380000000000006</v>
-      </c>
-      <c r="G130">
-        <v>30479.712</v>
-      </c>
-      <c r="H130">
-        <v>9915.99</v>
-      </c>
-      <c r="I130">
-        <v>20563.722000000002</v>
-      </c>
-      <c r="J130">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="K130">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A131">
-        <v>111.44</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>67</v>
       </c>
       <c r="B131">
-        <v>75.566999999999993</v>
-      </c>
-      <c r="C131">
-        <v>359.08</v>
-      </c>
-      <c r="D131">
-        <v>111.44</v>
-      </c>
-      <c r="E131">
-        <v>0</v>
-      </c>
-      <c r="F131">
-        <v>9.9789999999999992</v>
-      </c>
-      <c r="G131">
-        <v>22171.98</v>
-      </c>
-      <c r="H131">
-        <v>8858.0830000000005</v>
-      </c>
-      <c r="I131">
-        <v>13313.897000000001</v>
-      </c>
-      <c r="J131">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="K131">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A132">
-        <v>111.44</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>68</v>
       </c>
       <c r="B132">
-        <v>75.566999999999993</v>
-      </c>
-      <c r="C132">
-        <v>359.08</v>
-      </c>
-      <c r="D132">
-        <v>111.44</v>
-      </c>
-      <c r="E132">
-        <v>0</v>
-      </c>
-      <c r="F132">
-        <v>9.9789999999999992</v>
-      </c>
-      <c r="G132">
-        <v>22171.98</v>
-      </c>
-      <c r="H132">
-        <v>8858.0830000000005</v>
-      </c>
-      <c r="I132">
-        <v>13313.897000000001</v>
-      </c>
-      <c r="J132">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="K132">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A133">
-        <v>118.583</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>69</v>
       </c>
       <c r="B133">
-        <v>70.433000000000007</v>
-      </c>
-      <c r="C133">
-        <v>285.75599999999997</v>
-      </c>
-      <c r="D133">
-        <v>118.583</v>
-      </c>
-      <c r="E133">
-        <v>0</v>
-      </c>
-      <c r="F133">
-        <v>10.169</v>
-      </c>
-      <c r="G133">
-        <v>14328.38</v>
-      </c>
-      <c r="H133">
-        <v>7339.1490000000003</v>
-      </c>
-      <c r="I133">
-        <v>6989.2309999999998</v>
-      </c>
-      <c r="J133">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K133">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A134">
-        <v>118.583</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>12</v>
       </c>
       <c r="B134">
-        <v>70.433000000000007</v>
-      </c>
-      <c r="C134">
-        <v>285.75599999999997</v>
-      </c>
-      <c r="D134">
-        <v>118.583</v>
-      </c>
-      <c r="E134">
-        <v>0</v>
-      </c>
-      <c r="F134">
-        <v>10.169</v>
-      </c>
-      <c r="G134">
-        <v>14328.38</v>
-      </c>
-      <c r="H134">
-        <v>7339.1490000000003</v>
-      </c>
-      <c r="I134">
-        <v>6989.2309999999998</v>
-      </c>
-      <c r="J134">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K134">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A135">
-        <v>125.726</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>70</v>
       </c>
       <c r="B135">
-        <v>64.876999999999995</v>
-      </c>
-      <c r="C135">
-        <v>190.76400000000001</v>
-      </c>
-      <c r="D135">
-        <v>125.726</v>
-      </c>
-      <c r="E135">
-        <v>0</v>
-      </c>
-      <c r="F135">
-        <v>10.792999999999999</v>
-      </c>
-      <c r="G135">
-        <v>7743.9679999999998</v>
-      </c>
-      <c r="H135">
-        <v>5107.4960000000001</v>
-      </c>
-      <c r="I135">
-        <v>2636.4720000000002</v>
-      </c>
-      <c r="J135">
-        <v>0.08</v>
-      </c>
-      <c r="K135">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A136">
-        <v>125.726</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>71</v>
       </c>
       <c r="B136">
-        <v>64.876999999999995</v>
-      </c>
-      <c r="C136">
-        <v>190.76400000000001</v>
-      </c>
-      <c r="D136">
-        <v>125.726</v>
-      </c>
-      <c r="E136">
-        <v>0</v>
-      </c>
-      <c r="F136">
-        <v>10.792999999999999</v>
-      </c>
-      <c r="G136">
-        <v>7743.9679999999998</v>
-      </c>
-      <c r="H136">
-        <v>5107.4960000000001</v>
-      </c>
-      <c r="I136">
-        <v>2636.4720000000002</v>
-      </c>
-      <c r="J136">
-        <v>0.08</v>
-      </c>
-      <c r="K136">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A137">
-        <v>132.869</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>72</v>
       </c>
       <c r="B137">
-        <v>36.206000000000003</v>
-      </c>
-      <c r="C137">
-        <v>57.351999999999997</v>
-      </c>
-      <c r="D137">
-        <v>132.869</v>
-      </c>
-      <c r="E137">
-        <v>0</v>
-      </c>
-      <c r="F137">
-        <v>15.741</v>
-      </c>
-      <c r="G137">
-        <v>803.48900000000003</v>
-      </c>
-      <c r="H137">
-        <v>134.215</v>
-      </c>
-      <c r="I137">
-        <v>669.274</v>
-      </c>
-      <c r="J137">
-        <v>11.933</v>
-      </c>
-      <c r="K137">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A138">
-        <v>132.869</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>73</v>
       </c>
       <c r="B138">
-        <v>36.206000000000003</v>
-      </c>
-      <c r="C138">
-        <v>57.351999999999997</v>
-      </c>
-      <c r="D138">
-        <v>132.869</v>
-      </c>
-      <c r="E138">
-        <v>0</v>
-      </c>
-      <c r="F138">
-        <v>15.741</v>
-      </c>
-      <c r="G138">
-        <v>803.48900000000003</v>
-      </c>
-      <c r="H138">
-        <v>134.215</v>
-      </c>
-      <c r="I138">
-        <v>669.274</v>
-      </c>
-      <c r="J138">
-        <v>11.933</v>
-      </c>
-      <c r="K138">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A139">
-        <v>140.012</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>74</v>
       </c>
       <c r="B139">
-        <v>23.068000000000001</v>
-      </c>
-      <c r="C139">
-        <v>17.103999999999999</v>
-      </c>
-      <c r="D139">
-        <v>140.012</v>
-      </c>
-      <c r="E139">
-        <v>0</v>
-      </c>
-      <c r="F139">
-        <v>17.038</v>
-      </c>
-      <c r="G139">
-        <v>104.504</v>
-      </c>
-      <c r="H139">
-        <v>6.9820000000000002</v>
-      </c>
-      <c r="I139">
-        <v>97.522000000000006</v>
-      </c>
-      <c r="J139">
-        <v>15.53</v>
-      </c>
-      <c r="K139">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A140">
-        <v>140.012</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>75</v>
       </c>
       <c r="B140">
-        <v>23.068000000000001</v>
-      </c>
-      <c r="C140">
-        <v>17.103999999999999</v>
-      </c>
-      <c r="D140">
-        <v>140.012</v>
-      </c>
-      <c r="E140">
-        <v>0</v>
-      </c>
-      <c r="F140">
-        <v>17.038</v>
-      </c>
-      <c r="G140">
-        <v>104.504</v>
-      </c>
-      <c r="H140">
-        <v>6.9820000000000002</v>
-      </c>
-      <c r="I140">
-        <v>97.522000000000006</v>
-      </c>
-      <c r="J140">
-        <v>15.53</v>
-      </c>
-      <c r="K140">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A141">
-        <v>147.154</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>76</v>
       </c>
       <c r="B141">
-        <v>0</v>
-      </c>
-      <c r="C141">
-        <v>0</v>
-      </c>
-      <c r="D141">
-        <v>147.154</v>
-      </c>
-      <c r="E141">
-        <v>0</v>
-      </c>
-      <c r="F141">
-        <v>18</v>
-      </c>
-      <c r="G141">
-        <v>0</v>
-      </c>
-      <c r="H141">
-        <v>0</v>
-      </c>
-      <c r="I141">
-        <v>0</v>
-      </c>
-      <c r="J141">
-        <v>0</v>
-      </c>
-      <c r="K141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>59</v>
-      </c>
-      <c r="B143">
-        <v>139.43</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>60</v>
-      </c>
-      <c r="B144">
-        <v>33.299999999999997</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>61</v>
-      </c>
-      <c r="B145">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>62</v>
-      </c>
-      <c r="B146">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>63</v>
-      </c>
-      <c r="B147">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="B147" t="s">
+        <v>82</v>
+      </c>
+      <c r="C147" t="s">
+        <v>83</v>
+      </c>
+      <c r="D147" t="s">
+        <v>84</v>
+      </c>
+      <c r="E147" t="s">
+        <v>85</v>
+      </c>
+      <c r="F147" t="s">
+        <v>86</v>
+      </c>
+      <c r="G147" t="s">
+        <v>87</v>
+      </c>
+      <c r="H147" t="s">
+        <v>88</v>
+      </c>
+      <c r="I147" t="s">
+        <v>89</v>
+      </c>
+      <c r="J147" t="s">
+        <v>90</v>
+      </c>
+      <c r="K147" t="s">
+        <v>91</v>
+      </c>
+      <c r="L147" t="s">
+        <v>92</v>
+      </c>
+      <c r="M147" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>64</v>
-      </c>
-      <c r="B148">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>65</v>
-      </c>
-      <c r="B149">
-        <v>20914.55</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B150">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>7</v>
-      </c>
-      <c r="B151">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="B151" t="s">
+        <v>82</v>
+      </c>
+      <c r="C151" t="s">
+        <v>83</v>
+      </c>
+      <c r="D151" t="s">
+        <v>84</v>
+      </c>
+      <c r="E151" t="s">
+        <v>85</v>
+      </c>
+      <c r="F151" t="s">
+        <v>86</v>
+      </c>
+      <c r="G151" t="s">
+        <v>87</v>
+      </c>
+      <c r="H151" t="s">
+        <v>88</v>
+      </c>
+      <c r="I151" t="s">
+        <v>89</v>
+      </c>
+      <c r="J151" t="s">
+        <v>90</v>
+      </c>
+      <c r="K151" t="s">
+        <v>91</v>
+      </c>
+      <c r="L151" t="s">
+        <v>92</v>
+      </c>
+      <c r="M151" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>67</v>
-      </c>
-      <c r="B152">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
-        <v>68</v>
-      </c>
-      <c r="B153">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>69</v>
-      </c>
-      <c r="B154">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>12</v>
-      </c>
-      <c r="B155">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="B155" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>70</v>
-      </c>
-      <c r="B156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>71</v>
-      </c>
-      <c r="B157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
-        <v>72</v>
-      </c>
-      <c r="B158">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
-        <v>73</v>
-      </c>
-      <c r="B159">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
-        <v>74</v>
-      </c>
-      <c r="B160">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>75</v>
-      </c>
-      <c r="B161">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>76</v>
-      </c>
-      <c r="B162">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
-        <v>77</v>
-      </c>
-      <c r="B163">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
-        <v>81</v>
-      </c>
-      <c r="B168" t="s">
-        <v>82</v>
-      </c>
-      <c r="C168" t="s">
-        <v>83</v>
-      </c>
-      <c r="D168" t="s">
-        <v>84</v>
-      </c>
-      <c r="E168" t="s">
-        <v>85</v>
-      </c>
-      <c r="F168" t="s">
-        <v>86</v>
-      </c>
-      <c r="G168" t="s">
-        <v>87</v>
-      </c>
-      <c r="H168" t="s">
-        <v>88</v>
-      </c>
-      <c r="I168" t="s">
-        <v>89</v>
-      </c>
-      <c r="J168" t="s">
-        <v>90</v>
-      </c>
-      <c r="K168" t="s">
-        <v>91</v>
-      </c>
-      <c r="L168" t="s">
-        <v>92</v>
-      </c>
-      <c r="M168" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
-        <v>40</v>
-      </c>
-      <c r="B171">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
-        <v>81</v>
-      </c>
-      <c r="B172" t="s">
-        <v>82</v>
-      </c>
-      <c r="C172" t="s">
-        <v>83</v>
-      </c>
-      <c r="D172" t="s">
-        <v>84</v>
-      </c>
-      <c r="E172" t="s">
-        <v>85</v>
-      </c>
-      <c r="F172" t="s">
-        <v>86</v>
-      </c>
-      <c r="G172" t="s">
-        <v>87</v>
-      </c>
-      <c r="H172" t="s">
-        <v>88</v>
-      </c>
-      <c r="I172" t="s">
-        <v>89</v>
-      </c>
-      <c r="J172" t="s">
-        <v>90</v>
-      </c>
-      <c r="K172" t="s">
-        <v>91</v>
-      </c>
-      <c r="L172" t="s">
-        <v>92</v>
-      </c>
-      <c r="M172" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
-        <v>98</v>
-      </c>
-      <c r="B176" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A178" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vgm klopt t nu
</commit_message>
<xml_diff>
--- a/IP.xlsx
+++ b/IP.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomol\.spyder-py3\MT-1\IP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575719C0-35F3-481B-9417-1F61FC954675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C9B4F8-30D1-4C28-B192-3AA9DF546DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="VB schip van Goris" sheetId="1" r:id="rId1"/>
-    <sheet name="ik ben snelheid" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
-    <sheet name="Plaatdikte uitvogelen" sheetId="3" r:id="rId4"/>
-    <sheet name="Plaatdikte 2" sheetId="4" r:id="rId5"/>
-    <sheet name="Plaatdikte 3" sheetId="5" r:id="rId6"/>
-    <sheet name="Container" sheetId="7" r:id="rId7"/>
+    <sheet name="Container" sheetId="7" r:id="rId1"/>
+    <sheet name="VB schip van Goris" sheetId="1" r:id="rId2"/>
+    <sheet name="ik ben snelheid" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="Plaatdikte uitvogelen" sheetId="3" r:id="rId5"/>
+    <sheet name="Plaatdikte 2" sheetId="4" r:id="rId6"/>
+    <sheet name="Plaatdikte 3" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -794,6 +794,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4309077-2AFB-46BB-B10C-149960471737}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6">
+        <f>PRODUCT(B2:B4)</f>
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -5093,7 +5146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -9339,7 +9392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EC7652-81C6-4C07-80F9-5511A8282806}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9351,7 +9404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -13650,7 +13703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -17948,7 +18001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -22246,57 +22299,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4309077-2AFB-46BB-B10C-149960471737}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6">
-        <f>PRODUCT(B2:B4)</f>
-        <v>234</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
sheet 1 = lege conditie
</commit_message>
<xml_diff>
--- a/IP.xlsx
+++ b/IP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomol\.spyder-py3\MT-1\IP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/tlievaart_tudelft_nl/Documents/Q4/Integratie project 1/IP-26/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F252D4D-6ED0-4920-A2E1-D758FA73D69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{2F252D4D-6ED0-4920-A2E1-D758FA73D69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D803D709-72EE-49CD-8100-A825EF56E35B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Container" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="128">
   <si>
     <t>Loa  [m]</t>
   </si>
@@ -397,6 +397,30 @@
   </si>
   <si>
     <t>Deck is 15053 mm from WL</t>
+  </si>
+  <si>
+    <t>&lt;null&gt;</t>
+  </si>
+  <si>
+    <t>Traceback:</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Deck is 56.67 mm from WL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> in script</t>
+  </si>
+  <si>
+    <t>Runtime error SystemExitException: Position of LCB too far FWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  line 75</t>
+  </si>
+  <si>
+    <t>Deck is 18301 mm from WL</t>
   </si>
 </sst>
 </file>
@@ -843,8 +867,8 @@
   </sheetPr>
   <dimension ref="A1:M183"/>
   <sheetViews>
-    <sheetView topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="D127" sqref="D127"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5142,7 +5166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355A6046-8CDA-456D-8FE3-5FCCD8223AAC}">
   <dimension ref="A2:M183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -12054,12 +12078,1927 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EC7652-81C6-4C07-80F9-5511A8282806}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:M178"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection sqref="A1:M157"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>224.49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>34.997999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>20.998999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>173.905</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>96.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>136.72999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2.6989999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2.6989999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>2.6989999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>16.574999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>207.767</v>
+      </c>
+      <c r="C18">
+        <v>5.25</v>
+      </c>
+      <c r="D18">
+        <v>2.6989999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>8467.4779999999992</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>118833.591</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>129.14699999999999</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1.5189999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>110.782</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>11.617000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0.4975</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0.62939999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>4099.21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>125.771</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>2.6989999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>231065.277</v>
+      </c>
+      <c r="C29" s="11">
+        <v>7850900</v>
+      </c>
+      <c r="D29" s="11">
+        <v>8081900</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>4319.5479999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>65.760000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>163.87799999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44.613999999999997</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>52.896000000000001</v>
+      </c>
+      <c r="B45">
+        <v>11.532</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>61.177</v>
+      </c>
+      <c r="B46">
+        <v>29.31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>69.457999999999998</v>
+      </c>
+      <c r="B47">
+        <v>46.317999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>77.739000000000004</v>
+      </c>
+      <c r="B48">
+        <v>58.924999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>86.02</v>
+      </c>
+      <c r="B49">
+        <v>64.942999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>94.302000000000007</v>
+      </c>
+      <c r="B50">
+        <v>65.760000000000005</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>102.583</v>
+      </c>
+      <c r="B51">
+        <v>65.760000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>110.864</v>
+      </c>
+      <c r="B52">
+        <v>65.760000000000005</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>119.145</v>
+      </c>
+      <c r="B53">
+        <v>65.760000000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>127.42700000000001</v>
+      </c>
+      <c r="B54">
+        <v>65.760000000000005</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>135.708</v>
+      </c>
+      <c r="B55">
+        <v>65.753</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>143.989</v>
+      </c>
+      <c r="B56">
+        <v>65.311999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>152.27000000000001</v>
+      </c>
+      <c r="B57">
+        <v>63.267000000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>160.55099999999999</v>
+      </c>
+      <c r="B58">
+        <v>59.654000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>168.833</v>
+      </c>
+      <c r="B59">
+        <v>55.006</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>177.114</v>
+      </c>
+      <c r="B60">
+        <v>49.423999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>185.39500000000001</v>
+      </c>
+      <c r="B61">
+        <v>42.93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>193.67599999999999</v>
+      </c>
+      <c r="B62">
+        <v>35.500999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>201.95699999999999</v>
+      </c>
+      <c r="B63">
+        <v>27.074999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>210.239</v>
+      </c>
+      <c r="B64">
+        <v>16.946000000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>218.52</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>-4.49</v>
+      </c>
+      <c r="B69">
+        <v>165.779</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>6.2</v>
+      </c>
+      <c r="B70">
+        <v>229.09899999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>16.89</v>
+      </c>
+      <c r="B71">
+        <v>300.43400000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>27.58</v>
+      </c>
+      <c r="B72">
+        <v>376.91699999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>38.270000000000003</v>
+      </c>
+      <c r="B73">
+        <v>455.25900000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>48.96</v>
+      </c>
+      <c r="B74">
+        <v>531.28800000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>59.65</v>
+      </c>
+      <c r="B75">
+        <v>599.54399999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>70.34</v>
+      </c>
+      <c r="B76">
+        <v>653.03099999999995</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>81.03</v>
+      </c>
+      <c r="B77">
+        <v>684.23099999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>91.72</v>
+      </c>
+      <c r="B78">
+        <v>691.86599999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>102.41</v>
+      </c>
+      <c r="B79">
+        <v>691.87900000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>113.1</v>
+      </c>
+      <c r="B80">
+        <v>691.87900000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>123.79</v>
+      </c>
+      <c r="B81">
+        <v>691.87900000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>134.47999999999999</v>
+      </c>
+      <c r="B82">
+        <v>691.87</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>145.16999999999999</v>
+      </c>
+      <c r="B83">
+        <v>688.08</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>155.86000000000001</v>
+      </c>
+      <c r="B84">
+        <v>667.70699999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>166.55</v>
+      </c>
+      <c r="B85">
+        <v>631.41899999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>177.24</v>
+      </c>
+      <c r="B86">
+        <v>575.90300000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>187.93</v>
+      </c>
+      <c r="B87">
+        <v>496.43</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>198.62</v>
+      </c>
+      <c r="B88">
+        <v>389.137</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>209.31</v>
+      </c>
+      <c r="B89">
+        <v>250.517</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>220</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>41</v>
+      </c>
+      <c r="B93" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>46</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>40</v>
+      </c>
+      <c r="B97">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>47</v>
+      </c>
+      <c r="B98" t="s">
+        <v>48</v>
+      </c>
+      <c r="C98" t="s">
+        <v>49</v>
+      </c>
+      <c r="D98" t="s">
+        <v>50</v>
+      </c>
+      <c r="E98" t="s">
+        <v>51</v>
+      </c>
+      <c r="F98" t="s">
+        <v>52</v>
+      </c>
+      <c r="G98" t="s">
+        <v>53</v>
+      </c>
+      <c r="H98" t="s">
+        <v>54</v>
+      </c>
+      <c r="I98" t="s">
+        <v>55</v>
+      </c>
+      <c r="J98" t="s">
+        <v>56</v>
+      </c>
+      <c r="K98" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>-4.49</v>
+      </c>
+      <c r="B99">
+        <v>55.582999999999998</v>
+      </c>
+      <c r="C99">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="D99">
+        <v>-4.49</v>
+      </c>
+      <c r="E99">
+        <v>-2E-3</v>
+      </c>
+      <c r="F99">
+        <v>17.242000000000001</v>
+      </c>
+      <c r="G99">
+        <v>3.6749999999999998</v>
+      </c>
+      <c r="H99">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="I99">
+        <v>2.831</v>
+      </c>
+      <c r="J99">
+        <v>10.101000000000001</v>
+      </c>
+      <c r="K99">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>6.2</v>
+      </c>
+      <c r="B100">
+        <v>62.890999999999998</v>
+      </c>
+      <c r="C100">
+        <v>6.3E-2</v>
+      </c>
+      <c r="D100">
+        <v>6.2</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>16.303000000000001</v>
+      </c>
+      <c r="G100">
+        <v>5.4470000000000001</v>
+      </c>
+      <c r="H100">
+        <v>1.4490000000000001</v>
+      </c>
+      <c r="I100">
+        <v>3.9980000000000002</v>
+      </c>
+      <c r="J100">
+        <v>8.0259999999999998</v>
+      </c>
+      <c r="K100">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>16.89</v>
+      </c>
+      <c r="B101">
+        <v>70.253</v>
+      </c>
+      <c r="C101">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D101">
+        <v>16.89</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>15.38</v>
+      </c>
+      <c r="G101">
+        <v>7.7119999999999997</v>
+      </c>
+      <c r="H101">
+        <v>2.23</v>
+      </c>
+      <c r="I101">
+        <v>5.4820000000000002</v>
+      </c>
+      <c r="J101">
+        <v>6.3070000000000004</v>
+      </c>
+      <c r="K101">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>27.58</v>
+      </c>
+      <c r="B102">
+        <v>77.548000000000002</v>
+      </c>
+      <c r="C102">
+        <v>7.8E-2</v>
+      </c>
+      <c r="D102">
+        <v>27.58</v>
+      </c>
+      <c r="E102">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F102">
+        <v>14.487</v>
+      </c>
+      <c r="G102">
+        <v>10.474</v>
+      </c>
+      <c r="H102">
+        <v>3.1760000000000002</v>
+      </c>
+      <c r="I102">
+        <v>7.298</v>
+      </c>
+      <c r="J102">
+        <v>4.7869999999999999</v>
+      </c>
+      <c r="K102">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>38.270000000000003</v>
+      </c>
+      <c r="B103">
+        <v>84.533000000000001</v>
+      </c>
+      <c r="C103">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D103">
+        <v>38.270000000000003</v>
+      </c>
+      <c r="E103">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F103">
+        <v>13.667</v>
+      </c>
+      <c r="G103">
+        <v>13.609</v>
+      </c>
+      <c r="H103">
+        <v>4.2359999999999998</v>
+      </c>
+      <c r="I103">
+        <v>9.3719999999999999</v>
+      </c>
+      <c r="J103">
+        <v>3.427</v>
+      </c>
+      <c r="K103">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>48.96</v>
+      </c>
+      <c r="B104">
+        <v>90.924000000000007</v>
+      </c>
+      <c r="C104">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="D104">
+        <v>48.96</v>
+      </c>
+      <c r="E104">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F104">
+        <v>12.92</v>
+      </c>
+      <c r="G104">
+        <v>16.952000000000002</v>
+      </c>
+      <c r="H104">
+        <v>5.3550000000000004</v>
+      </c>
+      <c r="I104">
+        <v>11.597</v>
+      </c>
+      <c r="J104">
+        <v>2.2349999999999999</v>
+      </c>
+      <c r="K104">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>59.65</v>
+      </c>
+      <c r="B105">
+        <v>96.382000000000005</v>
+      </c>
+      <c r="C105">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D105">
+        <v>59.65</v>
+      </c>
+      <c r="E105">
+        <v>-2E-3</v>
+      </c>
+      <c r="F105">
+        <v>12.3</v>
+      </c>
+      <c r="G105">
+        <v>20.172000000000001</v>
+      </c>
+      <c r="H105">
+        <v>6.4210000000000003</v>
+      </c>
+      <c r="I105">
+        <v>13.75</v>
+      </c>
+      <c r="J105">
+        <v>1.2450000000000001</v>
+      </c>
+      <c r="K105">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>70.34</v>
+      </c>
+      <c r="B106">
+        <v>100.495</v>
+      </c>
+      <c r="C106">
+        <v>0.1</v>
+      </c>
+      <c r="D106">
+        <v>70.34</v>
+      </c>
+      <c r="E106">
+        <v>2E-3</v>
+      </c>
+      <c r="F106">
+        <v>11.835000000000001</v>
+      </c>
+      <c r="G106">
+        <v>22.847000000000001</v>
+      </c>
+      <c r="H106">
+        <v>7.2990000000000004</v>
+      </c>
+      <c r="I106">
+        <v>15.547000000000001</v>
+      </c>
+      <c r="J106">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="K106">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>81.03</v>
+      </c>
+      <c r="B107">
+        <v>102.833</v>
+      </c>
+      <c r="C107">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D107">
+        <v>81.03</v>
+      </c>
+      <c r="E107">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F107">
+        <v>11.577999999999999</v>
+      </c>
+      <c r="G107">
+        <v>24.468</v>
+      </c>
+      <c r="H107">
+        <v>7.819</v>
+      </c>
+      <c r="I107">
+        <v>16.648</v>
+      </c>
+      <c r="J107">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="K107">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>91.72</v>
+      </c>
+      <c r="B108">
+        <v>103.399</v>
+      </c>
+      <c r="C108">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D108">
+        <v>91.72</v>
+      </c>
+      <c r="E108">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F108">
+        <v>11.51</v>
+      </c>
+      <c r="G108">
+        <v>24.881</v>
+      </c>
+      <c r="H108">
+        <v>7.9539999999999997</v>
+      </c>
+      <c r="I108">
+        <v>16.925999999999998</v>
+      </c>
+      <c r="J108">
+        <v>-1E-3</v>
+      </c>
+      <c r="K108">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>102.41</v>
+      </c>
+      <c r="B109">
+        <v>103.4</v>
+      </c>
+      <c r="C109">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D109">
+        <v>102.41</v>
+      </c>
+      <c r="E109">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F109">
+        <v>11.51</v>
+      </c>
+      <c r="G109">
+        <v>24.88</v>
+      </c>
+      <c r="H109">
+        <v>7.9539999999999997</v>
+      </c>
+      <c r="I109">
+        <v>16.925000000000001</v>
+      </c>
+      <c r="J109">
+        <v>-1E-3</v>
+      </c>
+      <c r="K109">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>113.1</v>
+      </c>
+      <c r="B110">
+        <v>103.4</v>
+      </c>
+      <c r="C110">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D110">
+        <v>113.1</v>
+      </c>
+      <c r="E110">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F110">
+        <v>11.51</v>
+      </c>
+      <c r="G110">
+        <v>24.88</v>
+      </c>
+      <c r="H110">
+        <v>7.9539999999999997</v>
+      </c>
+      <c r="I110">
+        <v>16.925000000000001</v>
+      </c>
+      <c r="J110">
+        <v>-1E-3</v>
+      </c>
+      <c r="K110">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>123.79</v>
+      </c>
+      <c r="B111">
+        <v>103.4</v>
+      </c>
+      <c r="C111">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D111">
+        <v>123.79</v>
+      </c>
+      <c r="E111">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F111">
+        <v>11.51</v>
+      </c>
+      <c r="G111">
+        <v>24.88</v>
+      </c>
+      <c r="H111">
+        <v>7.9539999999999997</v>
+      </c>
+      <c r="I111">
+        <v>16.925000000000001</v>
+      </c>
+      <c r="J111">
+        <v>-1E-3</v>
+      </c>
+      <c r="K111">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>134.47999999999999</v>
+      </c>
+      <c r="B112">
+        <v>103.399</v>
+      </c>
+      <c r="C112">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D112">
+        <v>134.47999999999999</v>
+      </c>
+      <c r="E112">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F112">
+        <v>11.51</v>
+      </c>
+      <c r="G112">
+        <v>24.878</v>
+      </c>
+      <c r="H112">
+        <v>7.9539999999999997</v>
+      </c>
+      <c r="I112">
+        <v>16.923999999999999</v>
+      </c>
+      <c r="J112">
+        <v>-1E-3</v>
+      </c>
+      <c r="K112">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>145.16999999999999</v>
+      </c>
+      <c r="B113">
+        <v>103.054</v>
+      </c>
+      <c r="C113">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D113">
+        <v>145.16999999999999</v>
+      </c>
+      <c r="E113">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F113">
+        <v>11.519</v>
+      </c>
+      <c r="G113">
+        <v>24.613</v>
+      </c>
+      <c r="H113">
+        <v>7.9109999999999996</v>
+      </c>
+      <c r="I113">
+        <v>16.702000000000002</v>
+      </c>
+      <c r="J113">
+        <v>1E-3</v>
+      </c>
+      <c r="K113">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>155.86000000000001</v>
+      </c>
+      <c r="B114">
+        <v>101.18600000000001</v>
+      </c>
+      <c r="C114">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="D114">
+        <v>155.86000000000001</v>
+      </c>
+      <c r="E114">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="F114">
+        <v>11.551</v>
+      </c>
+      <c r="G114">
+        <v>23.338000000000001</v>
+      </c>
+      <c r="H114">
+        <v>7.6870000000000003</v>
+      </c>
+      <c r="I114">
+        <v>15.651</v>
+      </c>
+      <c r="J114">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K114">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>166.55</v>
+      </c>
+      <c r="B115">
+        <v>97.790999999999997</v>
+      </c>
+      <c r="C115">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="D115">
+        <v>166.55</v>
+      </c>
+      <c r="E115">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="F115">
+        <v>11.602</v>
+      </c>
+      <c r="G115">
+        <v>21.085000000000001</v>
+      </c>
+      <c r="H115">
+        <v>7.2830000000000004</v>
+      </c>
+      <c r="I115">
+        <v>13.802</v>
+      </c>
+      <c r="J115">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K115">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>177.24</v>
+      </c>
+      <c r="B116">
+        <v>92.504000000000005</v>
+      </c>
+      <c r="C116">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="D116">
+        <v>177.24</v>
+      </c>
+      <c r="E116">
+        <v>-2E-3</v>
+      </c>
+      <c r="F116">
+        <v>11.653</v>
+      </c>
+      <c r="G116">
+        <v>17.93</v>
+      </c>
+      <c r="H116">
+        <v>6.702</v>
+      </c>
+      <c r="I116">
+        <v>11.228</v>
+      </c>
+      <c r="J116">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="K116">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>187.93</v>
+      </c>
+      <c r="B117">
+        <v>84.906999999999996</v>
+      </c>
+      <c r="C117">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D117">
+        <v>187.93</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <v>11.691000000000001</v>
+      </c>
+      <c r="G117">
+        <v>13.917</v>
+      </c>
+      <c r="H117">
+        <v>5.8959999999999999</v>
+      </c>
+      <c r="I117">
+        <v>8.0210000000000008</v>
+      </c>
+      <c r="J117">
+        <v>1.9E-2</v>
+      </c>
+      <c r="K117">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>198.62</v>
+      </c>
+      <c r="B118">
+        <v>74.721999999999994</v>
+      </c>
+      <c r="C118">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D118">
+        <v>198.62</v>
+      </c>
+      <c r="E118">
+        <v>1E-3</v>
+      </c>
+      <c r="F118">
+        <v>11.705</v>
+      </c>
+      <c r="G118">
+        <v>9.4990000000000006</v>
+      </c>
+      <c r="H118">
+        <v>4.8470000000000004</v>
+      </c>
+      <c r="I118">
+        <v>4.6520000000000001</v>
+      </c>
+      <c r="J118">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K118">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>209.31</v>
+      </c>
+      <c r="B119">
+        <v>61.835000000000001</v>
+      </c>
+      <c r="C119">
+        <v>6.2E-2</v>
+      </c>
+      <c r="D119">
+        <v>209.31</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>11.663</v>
+      </c>
+      <c r="G119">
+        <v>5.3220000000000001</v>
+      </c>
+      <c r="H119">
+        <v>3.5339999999999998</v>
+      </c>
+      <c r="I119">
+        <v>1.7869999999999999</v>
+      </c>
+      <c r="J119">
+        <v>1E-3</v>
+      </c>
+      <c r="K119">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>220</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>220</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>14.34</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120">
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>59</v>
+      </c>
+      <c r="B122">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>60</v>
+      </c>
+      <c r="B123">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>61</v>
+      </c>
+      <c r="B124">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>62</v>
+      </c>
+      <c r="B125">
+        <v>2.6989999999999998</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>63</v>
+      </c>
+      <c r="B126">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>64</v>
+      </c>
+      <c r="B127">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>65</v>
+      </c>
+      <c r="B128">
+        <v>40260.036999999997</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>66</v>
+      </c>
+      <c r="B129">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>7</v>
+      </c>
+      <c r="B130">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>67</v>
+      </c>
+      <c r="B131">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>68</v>
+      </c>
+      <c r="B132">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>69</v>
+      </c>
+      <c r="B133">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>12</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>70</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>71</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>72</v>
+      </c>
+      <c r="B137">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>73</v>
+      </c>
+      <c r="B138">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>74</v>
+      </c>
+      <c r="B139">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>75</v>
+      </c>
+      <c r="B140">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>76</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>77</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>80</v>
+      </c>
+      <c r="B145" t="s">
+        <v>81</v>
+      </c>
+      <c r="C145" t="s">
+        <v>82</v>
+      </c>
+      <c r="D145" t="s">
+        <v>83</v>
+      </c>
+      <c r="E145" t="s">
+        <v>84</v>
+      </c>
+      <c r="F145" t="s">
+        <v>85</v>
+      </c>
+      <c r="G145" t="s">
+        <v>86</v>
+      </c>
+      <c r="H145" t="s">
+        <v>87</v>
+      </c>
+      <c r="I145" t="s">
+        <v>88</v>
+      </c>
+      <c r="J145" t="s">
+        <v>89</v>
+      </c>
+      <c r="K145" t="s">
+        <v>90</v>
+      </c>
+      <c r="L145" t="s">
+        <v>91</v>
+      </c>
+      <c r="M145" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>40</v>
+      </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>80</v>
+      </c>
+      <c r="B149" t="s">
+        <v>81</v>
+      </c>
+      <c r="C149" t="s">
+        <v>82</v>
+      </c>
+      <c r="D149" t="s">
+        <v>83</v>
+      </c>
+      <c r="E149" t="s">
+        <v>84</v>
+      </c>
+      <c r="F149" t="s">
+        <v>85</v>
+      </c>
+      <c r="G149" t="s">
+        <v>86</v>
+      </c>
+      <c r="H149" t="s">
+        <v>87</v>
+      </c>
+      <c r="I149" t="s">
+        <v>88</v>
+      </c>
+      <c r="J149" t="s">
+        <v>89</v>
+      </c>
+      <c r="K149" t="s">
+        <v>90</v>
+      </c>
+      <c r="L149" t="s">
+        <v>91</v>
+      </c>
+      <c r="M149" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>126</v>
+      </c>
+      <c r="B153" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>126</v>
+      </c>
+      <c r="B174" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>